<commit_message>
Fixed Youtube function and created Twitter Function.
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="608">
   <si>
     <t xml:space="preserve">Contact</t>
   </si>
@@ -1870,6 +1870,12 @@
   <si>
     <t xml:space="preserve">https://www.youtube.com/channel/Pewdiepie/videos</t>
   </si>
+  <si>
+    <t xml:space="preserve">Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/channel/Japan</t>
+  </si>
 </sst>
 </file>
 
@@ -1885,7 +1891,7 @@
     <numFmt numFmtId="170" formatCode="[H]:MM:SS"/>
     <numFmt numFmtId="171" formatCode="0%"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2121,13 +2127,6 @@
       <name val="Roboto"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="13">
@@ -2531,7 +2530,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2617,7 +2616,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="V9:Y11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11967,10 +11966,10 @@
   </sheetPr>
   <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="V11" activeCellId="0" sqref="V9:Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12513,18 +12512,10 @@
       <c r="U9" s="59" t="s">
         <v>548</v>
       </c>
-      <c r="V9" s="17" t="n">
-        <v>1.964</v>
-      </c>
-      <c r="W9" s="17" t="n">
-        <v>16</v>
-      </c>
-      <c r="X9" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="Y9" s="17" t="n">
-        <v>4.136</v>
-      </c>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
       <c r="Z9" s="17" t="n">
         <v>1</v>
       </c>
@@ -12597,18 +12588,10 @@
       <c r="U10" s="59" t="s">
         <v>555</v>
       </c>
-      <c r="V10" s="17" t="n">
-        <v>965</v>
-      </c>
-      <c r="W10" s="17" t="n">
-        <v>725</v>
-      </c>
-      <c r="X10" s="17" t="n">
-        <v>1527</v>
-      </c>
-      <c r="Y10" s="17" t="n">
-        <v>1.129</v>
-      </c>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
       <c r="Z10" s="17"/>
       <c r="AA10" s="17"/>
       <c r="AB10" s="17"/>
@@ -12621,7 +12604,7 @@
       <c r="AI10" s="17"/>
       <c r="AJ10" s="17"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
         <v>556</v>
       </c>
@@ -12673,18 +12656,10 @@
       <c r="U11" s="59" t="s">
         <v>561</v>
       </c>
-      <c r="V11" s="17" t="n">
-        <v>10.4</v>
-      </c>
-      <c r="W11" s="17" t="n">
-        <v>84</v>
-      </c>
-      <c r="X11" s="17" t="n">
-        <v>9</v>
-      </c>
-      <c r="Y11" s="17" t="n">
-        <v>1.102</v>
-      </c>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
       <c r="Z11" s="17" t="n">
         <v>0</v>
       </c>
@@ -12701,7 +12676,7 @@
       <c r="AI11" s="17"/>
       <c r="AJ11" s="17"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
         <v>562</v>
       </c>
@@ -12755,18 +12730,10 @@
       <c r="U12" s="59" t="s">
         <v>568</v>
       </c>
-      <c r="V12" s="17" t="n">
-        <v>658</v>
-      </c>
-      <c r="W12" s="17" t="n">
-        <v>1.402</v>
-      </c>
-      <c r="X12" s="17" t="n">
-        <v>33</v>
-      </c>
-      <c r="Y12" s="17" t="n">
-        <v>8.328</v>
-      </c>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
       <c r="Z12" s="17" t="n">
         <v>0</v>
       </c>
@@ -12787,7 +12754,7 @@
       <c r="AI12" s="17"/>
       <c r="AJ12" s="17"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
         <v>570</v>
       </c>
@@ -12841,18 +12808,10 @@
       <c r="U13" s="61" t="s">
         <v>576</v>
       </c>
-      <c r="V13" s="17" t="n">
-        <v>44</v>
-      </c>
-      <c r="W13" s="17" t="n">
-        <v>16</v>
-      </c>
-      <c r="X13" s="17" t="n">
-        <v>136</v>
-      </c>
-      <c r="Y13" s="17" t="n">
-        <v>772</v>
-      </c>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
       <c r="Z13" s="17"/>
       <c r="AA13" s="17"/>
       <c r="AB13" s="17"/>
@@ -12865,7 +12824,7 @@
       <c r="AI13" s="17"/>
       <c r="AJ13" s="17"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
         <v>577</v>
       </c>
@@ -12917,18 +12876,10 @@
       <c r="U14" s="61" t="s">
         <v>582</v>
       </c>
-      <c r="V14" s="17" t="n">
-        <v>806</v>
-      </c>
-      <c r="W14" s="17" t="n">
-        <v>259</v>
-      </c>
-      <c r="X14" s="17" t="n">
-        <v>467</v>
-      </c>
-      <c r="Y14" s="17" t="n">
-        <v>282</v>
-      </c>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
       <c r="Z14" s="17" t="n">
         <v>1</v>
       </c>
@@ -13201,7 +13152,21 @@
         <v>605</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="30" t="s">
+        <v>606</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30" t="s">
+        <v>607</v>
+      </c>
+    </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -14207,27 +14172,27 @@
     <hyperlink ref="E11" r:id="rId13" display="https://thetoyreviewervideos.com"/>
     <hyperlink ref="J11" r:id="rId14" display="https://www.youtube.com/user/TheToyReviewerVideos/videos"/>
     <hyperlink ref="N11" r:id="rId15" display="https://www.instagram.com/thetoyreviewer/"/>
-    <hyperlink ref="U11" r:id="rId16" display="https://www.instagram.com/thetoyreviewer/"/>
-    <hyperlink ref="J12" r:id="rId17" display="https://www.youtube.com/channel/UCE0cWpq6A-JQbn341mnfcvw/videos"/>
-    <hyperlink ref="N12" r:id="rId18" display="https://www.instagram.com/FamilyToyReview/"/>
-    <hyperlink ref="U12" r:id="rId19" display="https://twitter.com/FamilyToyReview"/>
-    <hyperlink ref="AB12" r:id="rId20" display="https://www.facebook.com/FamilyToyReview"/>
-    <hyperlink ref="E13" r:id="rId21" display="http://owenandliamstoyreview.com"/>
-    <hyperlink ref="J13" r:id="rId22" display="https://www.youtube.com/user/owenstoyreview/videos"/>
-    <hyperlink ref="N13" r:id="rId23" display="https://www.instagram.com/owenandliam/"/>
-    <hyperlink ref="U13" r:id="rId24" display="https://twitter.com/OwenAndLiam"/>
-    <hyperlink ref="J14" r:id="rId25" display="https://www.youtube.com/channel/UCOb3FSzZxslUzJeyuArwa4g"/>
-    <hyperlink ref="N14" r:id="rId26" display="https://www.instagram.com/jacestoyplayhouse/"/>
-    <hyperlink ref="U14" r:id="rId27" display="https://twitter.com/jacesplayhouse"/>
-    <hyperlink ref="AB14" r:id="rId28" display="https://www.facebook.com/Jaces-Toy-Playhouse-2267915886772395/?modal=admin_todo_tour"/>
-    <hyperlink ref="J15" r:id="rId29" display="https://www.youtube.com/channel/UCXSvZthhk3lLnblVH3x9MkA/videos"/>
-    <hyperlink ref="J16" r:id="rId30" display="https://www.youtube.com/channel/UCteJ7mTMxzywmIF1o-CaUkA/videos"/>
-    <hyperlink ref="N16" r:id="rId31" display="https://www.instagram.com/mikey_likes_it1/"/>
-    <hyperlink ref="AB16" r:id="rId32" display="https://www.facebook.com/mikeylikesityoutube"/>
-    <hyperlink ref="J17" r:id="rId33" display="https://www.youtube.com/channel/UCw2Hb9NBLH6nG5HmIw_UZ8w/videos"/>
-    <hyperlink ref="N17" r:id="rId34" display="https://www.instagram.com/planetserenitychannel/"/>
-    <hyperlink ref="U17" r:id="rId35" display="https://twitter.com/PlanettSerenity"/>
-    <hyperlink ref="J19" r:id="rId36" display="https://www.youtube.com/channel/Pewdiepie/"/>
+    <hyperlink ref="J12" r:id="rId16" display="https://www.youtube.com/channel/UCE0cWpq6A-JQbn341mnfcvw/videos"/>
+    <hyperlink ref="N12" r:id="rId17" display="https://www.instagram.com/FamilyToyReview/"/>
+    <hyperlink ref="U12" r:id="rId18" display="https://twitter.com/FamilyToyReview"/>
+    <hyperlink ref="AB12" r:id="rId19" display="https://www.facebook.com/FamilyToyReview"/>
+    <hyperlink ref="E13" r:id="rId20" display="http://owenandliamstoyreview.com"/>
+    <hyperlink ref="J13" r:id="rId21" display="https://www.youtube.com/user/owenstoyreview/videos"/>
+    <hyperlink ref="N13" r:id="rId22" display="https://www.instagram.com/owenandliam/"/>
+    <hyperlink ref="U13" r:id="rId23" display="https://twitter.com/OwenAndLiam"/>
+    <hyperlink ref="J14" r:id="rId24" display="https://www.youtube.com/channel/UCOb3FSzZxslUzJeyuArwa4g"/>
+    <hyperlink ref="N14" r:id="rId25" display="https://www.instagram.com/jacestoyplayhouse/"/>
+    <hyperlink ref="U14" r:id="rId26" display="https://twitter.com/jacesplayhouse"/>
+    <hyperlink ref="AB14" r:id="rId27" display="https://www.facebook.com/Jaces-Toy-Playhouse-2267915886772395/?modal=admin_todo_tour"/>
+    <hyperlink ref="J15" r:id="rId28" display="https://www.youtube.com/channel/UCXSvZthhk3lLnblVH3x9MkA/videos"/>
+    <hyperlink ref="J16" r:id="rId29" display="https://www.youtube.com/channel/UCteJ7mTMxzywmIF1o-CaUkA/videos"/>
+    <hyperlink ref="N16" r:id="rId30" display="https://www.instagram.com/mikey_likes_it1/"/>
+    <hyperlink ref="AB16" r:id="rId31" display="https://www.facebook.com/mikeylikesityoutube"/>
+    <hyperlink ref="J17" r:id="rId32" display="https://www.youtube.com/channel/UCw2Hb9NBLH6nG5HmIw_UZ8w/videos"/>
+    <hyperlink ref="N17" r:id="rId33" display="https://www.instagram.com/planetserenitychannel/"/>
+    <hyperlink ref="U17" r:id="rId34" display="https://twitter.com/PlanettSerenity"/>
+    <hyperlink ref="J19" r:id="rId35" display="https://www.youtube.com/channel/Pewdiepie/videos"/>
+    <hyperlink ref="J20" r:id="rId36" display="https://www.youtube.com/channel/Japan"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>